<commit_message>
Base ETL ,updated schema and Examples
</commit_message>
<xml_diff>
--- a/Schema/DB_scheme.xlsx
+++ b/Schema/DB_scheme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksam432/Documents/Work/WP3/Databases/schema/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksam432/Documents/GitHub/WP3/Schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7415867D-D3A1-AD42-9EF5-4B59A9BAD4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E99E980-1498-4547-9697-6E574A24DC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="336">
   <si>
     <t>PROJET :</t>
   </si>
@@ -853,9 +853,6 @@
     <t>pair_style</t>
   </si>
   <si>
-    <t>compatability</t>
-  </si>
-  <si>
     <t>The description on choice of hyperparameter settings</t>
   </si>
   <si>
@@ -970,9 +967,6 @@
     <t>Kpoint method and grid</t>
   </si>
   <si>
-    <t>[ev/A]</t>
-  </si>
-  <si>
     <t>Electronic convergence threshold</t>
   </si>
   <si>
@@ -1049,6 +1043,9 @@
   </si>
   <si>
     <t>["RDF","Phonon"]</t>
+  </si>
+  <si>
+    <t>atomistic_engines</t>
   </si>
 </sst>
 </file>
@@ -2094,33 +2091,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2157,6 +2127,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2591,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2616,21 +2613,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="117" t="s">
+      <c r="C2" s="131"/>
+      <c r="D2" s="132" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -3365,7 +3362,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>271</v>
+        <v>335</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>176</v>
@@ -3416,7 +3413,7 @@
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
       <c r="M29" s="21" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3434,7 +3431,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -3472,7 +3469,7 @@
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
       <c r="M31" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N31" t="s">
         <v>19</v>
@@ -3504,7 +3501,7 @@
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
       <c r="M32" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N32" t="s">
         <v>19</v>
@@ -3534,7 +3531,7 @@
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
       <c r="M33" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3543,7 +3540,7 @@
         <v>194</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D34" s="17">
         <v>1</v>
@@ -3565,7 +3562,7 @@
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3586,7 +3583,7 @@
         <v>18</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="23"/>
@@ -3596,7 +3593,7 @@
       <c r="K35" s="18"/>
       <c r="L35" s="18"/>
       <c r="M35" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3617,7 +3614,7 @@
         <v>18</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="18"/>
@@ -3627,7 +3624,7 @@
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3648,7 +3645,7 @@
         <v>15</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H37" s="18"/>
       <c r="I37" s="18"/>
@@ -3658,15 +3655,15 @@
       <c r="K37" s="18"/>
       <c r="L37" s="18"/>
       <c r="M37" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:13" s="109" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="125"/>
+      <c r="A38" s="116"/>
       <c r="B38" s="110" t="s">
         <v>194</v>
       </c>
-      <c r="C38" s="126" t="s">
+      <c r="C38" s="117" t="s">
         <v>202</v>
       </c>
       <c r="D38" s="112">
@@ -3675,11 +3672,11 @@
       <c r="E38" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="127" t="s">
+      <c r="F38" s="118" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H38" s="113"/>
       <c r="I38" s="113"/>
@@ -3689,32 +3686,32 @@
       <c r="K38" s="113"/>
       <c r="L38" s="113"/>
       <c r="M38" s="21" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" s="133" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="128"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="119"/>
       <c r="B39" s="110" t="s">
         <v>203</v>
       </c>
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="131">
-        <v>1</v>
-      </c>
-      <c r="E39" s="130" t="s">
+      <c r="D39" s="122">
+        <v>1</v>
+      </c>
+      <c r="E39" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="132" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="132"/>
-      <c r="H39" s="132"/>
-      <c r="I39" s="132"/>
-      <c r="J39" s="132"/>
-      <c r="K39" s="132"/>
-      <c r="L39" s="132"/>
+      <c r="F39" s="123" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="123"/>
+      <c r="H39" s="123"/>
+      <c r="I39" s="123"/>
+      <c r="J39" s="123"/>
+      <c r="K39" s="123"/>
+      <c r="L39" s="123"/>
       <c r="M39" s="20" t="s">
         <v>16</v>
       </c>
@@ -3745,7 +3742,7 @@
       <c r="K40" s="18"/>
       <c r="L40" s="18"/>
       <c r="M40" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3774,7 +3771,7 @@
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
       <c r="M41" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3783,7 +3780,7 @@
         <v>203</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D42" s="17">
         <v>1</v>
@@ -3802,10 +3799,10 @@
       </c>
       <c r="K42" s="18"/>
       <c r="L42" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="M42" s="19" t="s">
         <v>292</v>
-      </c>
-      <c r="M42" s="19" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3814,7 +3811,7 @@
         <v>203</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D43" s="17">
         <v>1</v>
@@ -3834,7 +3831,7 @@
       <c r="K43" s="18"/>
       <c r="L43" s="18"/>
       <c r="M43" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3843,7 +3840,7 @@
         <v>203</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D44" s="17">
         <v>1</v>
@@ -3863,7 +3860,7 @@
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
       <c r="M44" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -3892,7 +3889,7 @@
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
       <c r="M45" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -3921,7 +3918,7 @@
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
       <c r="M46" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:13" s="109" customFormat="1" x14ac:dyDescent="0.2">
@@ -3950,8 +3947,8 @@
       </c>
       <c r="K47" s="113"/>
       <c r="L47" s="113"/>
-      <c r="M47" s="134" t="s">
-        <v>281</v>
+      <c r="M47" s="125" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -3981,7 +3978,7 @@
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
       <c r="M48" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.2">
@@ -4001,7 +3998,7 @@
         <v>18</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
@@ -4011,7 +4008,7 @@
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
       <c r="M49" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.2">
@@ -4031,7 +4028,7 @@
         <v>18</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="18"/>
@@ -4041,7 +4038,7 @@
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
       <c r="M50" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.2">
@@ -4069,7 +4066,7 @@
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
       <c r="M51" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.2">
@@ -4097,7 +4094,7 @@
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
       <c r="M52" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.2">
@@ -4123,29 +4120,31 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
       <c r="M53" s="27" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" s="133" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="129" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B54" s="120" t="s">
         <v>210</v>
       </c>
-      <c r="C54" s="130" t="s">
+      <c r="C54" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="131">
-        <v>1</v>
-      </c>
-      <c r="E54" s="130" t="s">
+      <c r="D54" s="122">
+        <v>1</v>
+      </c>
+      <c r="E54" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="132"/>
-      <c r="G54" s="132"/>
-      <c r="H54" s="132"/>
-      <c r="I54" s="132"/>
-      <c r="J54" s="132"/>
-      <c r="K54" s="132"/>
-      <c r="L54" s="132"/>
+      <c r="F54" s="123" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="123"/>
+      <c r="H54" s="123"/>
+      <c r="I54" s="123"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="123"/>
       <c r="M54" s="20" t="s">
         <v>16</v>
       </c>
@@ -4155,7 +4154,7 @@
         <v>210</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D55" s="17">
         <v>1</v>
@@ -4175,7 +4174,7 @@
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
       <c r="M55" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.2">
@@ -4203,7 +4202,7 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
       <c r="M56" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.2">
@@ -4230,10 +4229,10 @@
       </c>
       <c r="K57" s="18"/>
       <c r="L57" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M57" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.2">
@@ -4261,7 +4260,7 @@
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
       <c r="M58" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.2">
@@ -4281,7 +4280,7 @@
         <v>15</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H59" s="18"/>
       <c r="I59" s="18"/>
@@ -4291,7 +4290,7 @@
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
       <c r="M59" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
@@ -4311,7 +4310,7 @@
         <v>15</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H60" s="18"/>
       <c r="I60" s="18"/>
@@ -4321,7 +4320,7 @@
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
       <c r="M60" s="27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
@@ -4349,7 +4348,7 @@
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
       <c r="M61" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.2">
@@ -4377,7 +4376,7 @@
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
       <c r="M62" s="27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.2">
@@ -4405,7 +4404,7 @@
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
       <c r="M63" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.2">
@@ -4425,7 +4424,7 @@
         <v>15</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H64" s="18"/>
       <c r="I64" s="18"/>
@@ -4435,7 +4434,7 @@
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
       <c r="M64" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.2">
@@ -4455,7 +4454,7 @@
         <v>15</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
@@ -4465,29 +4464,31 @@
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
       <c r="M65" s="16" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" s="133" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" s="110" t="s">
         <v>219</v>
       </c>
-      <c r="C66" s="130" t="s">
+      <c r="C66" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="D66" s="131">
-        <v>1</v>
-      </c>
-      <c r="E66" s="130" t="s">
+      <c r="D66" s="122">
+        <v>1</v>
+      </c>
+      <c r="E66" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="132"/>
-      <c r="G66" s="132"/>
-      <c r="H66" s="132"/>
-      <c r="I66" s="132"/>
-      <c r="J66" s="132"/>
-      <c r="K66" s="132"/>
-      <c r="L66" s="132"/>
+      <c r="F66" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="123"/>
+      <c r="H66" s="123"/>
+      <c r="I66" s="123"/>
+      <c r="J66" s="123"/>
+      <c r="K66" s="123"/>
+      <c r="L66" s="123"/>
       <c r="M66" s="20" t="s">
         <v>16</v>
       </c>
@@ -4515,7 +4516,7 @@
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
       <c r="M67" s="27" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.2">
@@ -4541,7 +4542,7 @@
       <c r="K68" s="18"/>
       <c r="L68" s="18"/>
       <c r="M68" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.2">
@@ -4569,7 +4570,7 @@
       <c r="K69" s="18"/>
       <c r="L69" s="18"/>
       <c r="M69" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.2">
@@ -4594,10 +4595,10 @@
       <c r="J70" s="18"/>
       <c r="K70" s="18"/>
       <c r="L70" s="18" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M70" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.2">
@@ -4623,7 +4624,7 @@
       <c r="K71" s="18"/>
       <c r="L71" s="18"/>
       <c r="M71" s="27" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.2">
@@ -4651,7 +4652,7 @@
       <c r="K72" s="18"/>
       <c r="L72" s="18"/>
       <c r="M72" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.2">
@@ -4677,7 +4678,7 @@
       <c r="K73" s="18"/>
       <c r="L73" s="18"/>
       <c r="M73" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.2">
@@ -4703,31 +4704,31 @@
       <c r="K74" s="18"/>
       <c r="L74" s="18"/>
       <c r="M74" s="16" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" s="135" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" s="126" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B75" s="110" t="s">
         <v>226</v>
       </c>
-      <c r="C75" s="136" t="s">
+      <c r="C75" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D75" s="137">
-        <v>1</v>
-      </c>
-      <c r="E75" s="136" t="s">
+      <c r="D75" s="128">
+        <v>1</v>
+      </c>
+      <c r="E75" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="F75" s="138" t="s">
-        <v>18</v>
-      </c>
-      <c r="G75" s="138"/>
-      <c r="H75" s="138"/>
-      <c r="I75" s="138"/>
-      <c r="J75" s="138"/>
-      <c r="K75" s="138"/>
-      <c r="L75" s="138"/>
+      <c r="F75" s="129" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75" s="129"/>
+      <c r="H75" s="129"/>
+      <c r="I75" s="129"/>
+      <c r="J75" s="129"/>
+      <c r="K75" s="129"/>
+      <c r="L75" s="129"/>
       <c r="M75" s="20" t="s">
         <v>16</v>
       </c>
@@ -4751,13 +4752,13 @@
       <c r="G76" s="18"/>
       <c r="H76" s="18"/>
       <c r="I76" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J76" s="18"/>
       <c r="K76" s="18"/>
       <c r="L76" s="18"/>
       <c r="M76" s="16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.2">
@@ -4765,7 +4766,7 @@
         <v>226</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D77" s="17">
         <v>1</v>
@@ -4785,7 +4786,7 @@
       <c r="K77" s="18"/>
       <c r="L77" s="18"/>
       <c r="M77" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.2">
@@ -4793,7 +4794,7 @@
         <v>226</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D78" s="17">
         <v>1</v>
@@ -4811,7 +4812,7 @@
       <c r="K78" s="18"/>
       <c r="L78" s="18"/>
       <c r="M78" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.2">
@@ -4837,7 +4838,7 @@
       <c r="K79" s="18"/>
       <c r="L79" s="18"/>
       <c r="M79" s="27" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.2">
@@ -4863,32 +4864,32 @@
       <c r="K80" s="18"/>
       <c r="L80" s="18"/>
       <c r="M80" s="16" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13" s="135" customFormat="1" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" s="126" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="110" t="s">
         <v>267</v>
       </c>
-      <c r="C81" s="136" t="s">
+      <c r="C81" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D81" s="137">
-        <v>1</v>
-      </c>
-      <c r="E81" s="136" t="s">
+      <c r="D81" s="128">
+        <v>1</v>
+      </c>
+      <c r="E81" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="F81" s="138" t="s">
+      <c r="F81" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="G81" s="138"/>
-      <c r="H81" s="138"/>
-      <c r="I81" s="138"/>
-      <c r="J81" s="138"/>
-      <c r="K81" s="138"/>
-      <c r="L81" s="138"/>
-      <c r="M81" s="139" t="s">
+      <c r="G81" s="129"/>
+      <c r="H81" s="129"/>
+      <c r="I81" s="129"/>
+      <c r="J81" s="129"/>
+      <c r="K81" s="129"/>
+      <c r="L81" s="129"/>
+      <c r="M81" s="130" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4897,7 +4898,7 @@
         <v>267</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D82" s="17">
         <v>1</v>
@@ -4917,7 +4918,7 @@
       <c r="K82" s="18"/>
       <c r="L82" s="18"/>
       <c r="M82" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.2">
@@ -4945,7 +4946,7 @@
       <c r="K83" s="18"/>
       <c r="L83" s="18"/>
       <c r="M83" s="16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.2">
@@ -4973,7 +4974,7 @@
       <c r="K84" s="18"/>
       <c r="L84" s="18"/>
       <c r="M84" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.2">
@@ -5001,7 +5002,7 @@
       <c r="K85" s="18"/>
       <c r="L85" s="18"/>
       <c r="M85" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -6213,37 +6214,37 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="118" t="s">
+      <c r="B47" s="133" t="s">
         <v>126</v>
       </c>
-      <c r="C47" s="118"/>
-      <c r="D47" s="118"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
-      <c r="H47" s="119" t="s">
+      <c r="C47" s="133"/>
+      <c r="D47" s="133"/>
+      <c r="E47" s="133"/>
+      <c r="F47" s="133"/>
+      <c r="H47" s="134" t="s">
         <v>127</v>
       </c>
-      <c r="I47" s="119"/>
+      <c r="I47" s="134"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="118"/>
-      <c r="C48" s="118"/>
-      <c r="D48" s="118"/>
-      <c r="E48" s="118"/>
-      <c r="F48" s="118"/>
-      <c r="H48" s="119"/>
-      <c r="I48" s="119"/>
+      <c r="B48" s="133"/>
+      <c r="C48" s="133"/>
+      <c r="D48" s="133"/>
+      <c r="E48" s="133"/>
+      <c r="F48" s="133"/>
+      <c r="H48" s="134"/>
+      <c r="I48" s="134"/>
     </row>
     <row r="49" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="C49" s="120" t="s">
+      <c r="C49" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="120"/>
-      <c r="E49" s="120"/>
-      <c r="F49" s="120"/>
+      <c r="D49" s="135"/>
+      <c r="E49" s="135"/>
+      <c r="F49" s="135"/>
       <c r="H49" s="80" t="s">
         <v>129</v>
       </c>
@@ -6255,12 +6256,12 @@
       <c r="B50" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="121" t="s">
+      <c r="C50" s="136" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="121"/>
-      <c r="E50" s="121"/>
-      <c r="F50" s="121"/>
+      <c r="D50" s="136"/>
+      <c r="E50" s="136"/>
+      <c r="F50" s="136"/>
       <c r="H50" s="83" t="s">
         <v>53</v>
       </c>
@@ -6272,12 +6273,12 @@
       <c r="B51" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="122" t="s">
+      <c r="C51" s="137" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="122"/>
+      <c r="D51" s="137"/>
+      <c r="E51" s="137"/>
+      <c r="F51" s="137"/>
       <c r="H51" s="86" t="s">
         <v>75</v>
       </c>
@@ -6289,12 +6290,12 @@
       <c r="B52" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="122" t="s">
+      <c r="C52" s="137" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="122"/>
-      <c r="E52" s="122"/>
-      <c r="F52" s="122"/>
+      <c r="D52" s="137"/>
+      <c r="E52" s="137"/>
+      <c r="F52" s="137"/>
       <c r="H52" s="88" t="s">
         <v>136</v>
       </c>
@@ -6306,12 +6307,12 @@
       <c r="B53" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="123" t="s">
+      <c r="C53" s="138" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="123"/>
-      <c r="E53" s="123"/>
-      <c r="F53" s="123"/>
+      <c r="D53" s="138"/>
+      <c r="E53" s="138"/>
+      <c r="F53" s="138"/>
       <c r="H53" s="88" t="s">
         <v>86</v>
       </c>
@@ -6323,12 +6324,12 @@
       <c r="B54" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="122" t="s">
+      <c r="C54" s="137" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="122"/>
-      <c r="E54" s="122"/>
-      <c r="F54" s="122"/>
+      <c r="D54" s="137"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="137"/>
       <c r="H54" s="88" t="s">
         <v>60</v>
       </c>
@@ -6340,12 +6341,12 @@
       <c r="B55" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="123" t="s">
+      <c r="C55" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D55" s="123"/>
-      <c r="E55" s="123"/>
-      <c r="F55" s="123"/>
+      <c r="D55" s="138"/>
+      <c r="E55" s="138"/>
+      <c r="F55" s="138"/>
       <c r="H55" s="90" t="s">
         <v>119</v>
       </c>
@@ -6357,67 +6358,67 @@
       <c r="B56" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="122" t="s">
+      <c r="C56" s="137" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="122"/>
-      <c r="E56" s="122"/>
-      <c r="F56" s="122"/>
+      <c r="D56" s="137"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="137"/>
     </row>
     <row r="57" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="122" t="s">
+      <c r="C57" s="137" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="122"/>
-      <c r="E57" s="122"/>
-      <c r="F57" s="122"/>
+      <c r="D57" s="137"/>
+      <c r="E57" s="137"/>
+      <c r="F57" s="137"/>
     </row>
     <row r="58" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="122" t="s">
+      <c r="C58" s="137" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="122"/>
-      <c r="E58" s="122"/>
-      <c r="F58" s="122"/>
+      <c r="D58" s="137"/>
+      <c r="E58" s="137"/>
+      <c r="F58" s="137"/>
     </row>
     <row r="59" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="122" t="s">
+      <c r="C59" s="137" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="122"/>
-      <c r="E59" s="122"/>
-      <c r="F59" s="122"/>
+      <c r="D59" s="137"/>
+      <c r="E59" s="137"/>
+      <c r="F59" s="137"/>
     </row>
     <row r="60" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="122" t="s">
+      <c r="C60" s="137" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="122"/>
-      <c r="E60" s="122"/>
-      <c r="F60" s="122"/>
+      <c r="D60" s="137"/>
+      <c r="E60" s="137"/>
+      <c r="F60" s="137"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="124" t="s">
+      <c r="C61" s="139" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="124"/>
-      <c r="E61" s="124"/>
-      <c r="F61" s="124"/>
+      <c r="D61" s="139"/>
+      <c r="E61" s="139"/>
+      <c r="F61" s="139"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="EAttMbwrYpwG6akiV7biz2nw7wlXtTooCxJogsSt7negKq0wKQ9sygPbVeHZ99cgmdNfAtLu9NnPC64y/Uaw7A==" saltValue="FJhchlgDftI44klS+XpFDg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
Updated schema to include models for long range einteractions and introdcution of labels
</commit_message>
<xml_diff>
--- a/Schema/DB_scheme.xlsx
+++ b/Schema/DB_scheme.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksam432/Documents/GitHub/WP3/Schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E99E980-1498-4547-9697-6E574A24DC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0B2450-7ADC-8147-987E-B4C2DF8050F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="338">
   <si>
     <t>PROJET :</t>
   </si>
@@ -586,9 +586,6 @@
     <t>['scratch','fine-tune']</t>
   </si>
   <si>
-    <t>pretrained_variant</t>
-  </si>
-  <si>
     <t>Version of software used</t>
   </si>
   <si>
@@ -628,9 +625,6 @@
     <t>model_id</t>
   </si>
   <si>
-    <t>no_of_params</t>
-  </si>
-  <si>
     <t>config_file_path</t>
   </si>
   <si>
@@ -781,12 +775,6 @@
     <t xml:space="preserve">The type of MLIP  </t>
   </si>
   <si>
-    <t>The category of pre-trained model</t>
-  </si>
-  <si>
-    <t>['none','OFF','xxx']</t>
-  </si>
-  <si>
     <t>The doi for the publication of the model</t>
   </si>
   <si>
@@ -856,9 +844,6 @@
     <t>The description on choice of hyperparameter settings</t>
   </si>
   <si>
-    <t>Number of parameters in the model</t>
-  </si>
-  <si>
     <t>The path to metadata file or downloadable link</t>
   </si>
   <si>
@@ -874,9 +859,6 @@
     <t>The root mean square error on forces for  validation/test set</t>
   </si>
   <si>
-    <t>[eV/atom]</t>
-  </si>
-  <si>
     <t>[eV/A]</t>
   </si>
   <si>
@@ -913,30 +895,18 @@
     <t>The ellemt coverage in the dataset</t>
   </si>
   <si>
-    <t>["train,"val"]</t>
-  </si>
-  <si>
     <t>The type of dataset ( training-set or validation-set)</t>
   </si>
   <si>
-    <t>The targeted system for the dataset (eg: Materials, liquids,Organic}</t>
-  </si>
-  <si>
     <t>The date of submission</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>The link to the dataset (eg: hosted on some other website)</t>
   </si>
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>target_system</t>
-  </si>
-  <si>
     <t>software</t>
   </si>
   <si>
@@ -1046,6 +1016,42 @@
   </si>
   <si>
     <t>atomistic_engines</t>
+  </si>
+  <si>
+    <t>source_link</t>
+  </si>
+  <si>
+    <t>[meV/A]</t>
+  </si>
+  <si>
+    <t>[meV/atom]</t>
+  </si>
+  <si>
+    <t>["training","test","val"]</t>
+  </si>
+  <si>
+    <t>The category of pre-trained model ( type &amp; size )</t>
+  </si>
+  <si>
+    <t>long_range_interaction</t>
+  </si>
+  <si>
+    <t>test_set</t>
+  </si>
+  <si>
+    <t>The test set details</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>The labelsfor the dataset (eg: Materials, liquids,Organic}</t>
+  </si>
+  <si>
+    <t>The model has electrostatics taken into account</t>
+  </si>
+  <si>
+    <t>pretrained</t>
   </si>
 </sst>
 </file>
@@ -1770,7 +1776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2127,6 +2133,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2586,10 +2595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:N85"/>
+  <dimension ref="A2:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82:C85"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2613,21 +2622,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="132" t="s">
+      <c r="C2" s="132"/>
+      <c r="D2" s="133" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="132"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -2714,7 +2723,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
@@ -2745,7 +2754,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
@@ -2776,7 +2785,7 @@
       <c r="H9" s="107"/>
       <c r="I9" s="107"/>
       <c r="J9" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K9" s="107" t="s">
         <v>23</v>
@@ -2788,7 +2797,7 @@
         <v>173</v>
       </c>
       <c r="N9" s="104" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="17" x14ac:dyDescent="0.2">
@@ -2811,7 +2820,7 @@
       <c r="H10" s="107"/>
       <c r="I10" s="107"/>
       <c r="J10" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K10" s="107"/>
       <c r="L10" s="107"/>
@@ -2819,7 +2828,7 @@
         <v>177</v>
       </c>
       <c r="N10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="17" x14ac:dyDescent="0.2">
@@ -2842,19 +2851,19 @@
       <c r="H11" s="107"/>
       <c r="I11" s="107"/>
       <c r="J11" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K11" s="107" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="107" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M11" s="108" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N11" s="104" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -2862,13 +2871,13 @@
         <v>60</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>182</v>
+        <v>337</v>
       </c>
       <c r="D12" s="17">
         <v>1</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>15</v>
@@ -2877,19 +2886,15 @@
       <c r="H12" s="18"/>
       <c r="I12" s="16"/>
       <c r="J12" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="N12" s="115" t="s">
         <v>248</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="N12" s="115" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -2897,13 +2902,13 @@
         <v>60</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>180</v>
+        <v>331</v>
       </c>
       <c r="D13" s="17">
         <v>1</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>18</v>
@@ -2912,52 +2917,53 @@
       <c r="H13" s="18"/>
       <c r="I13" s="16"/>
       <c r="J13" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>181</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
       <c r="M13" s="16" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+      <c r="N13" s="131"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D14" s="17">
         <v>1</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15" s="17">
         <v>1</v>
@@ -2966,26 +2972,26 @@
         <v>14</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
-      <c r="I15" s="16"/>
+      <c r="I15" s="18"/>
       <c r="J15" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
-      <c r="M15" s="16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="M15" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D16" s="17">
         <v>1</v>
@@ -2998,17 +3004,14 @@
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="I16" s="16"/>
       <c r="J16" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
-      <c r="M16" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="N16" t="s">
-        <v>20</v>
+      <c r="M16" s="16" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3016,7 +3019,7 @@
         <v>60</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="D17" s="17">
         <v>1</v>
@@ -3025,119 +3028,115 @@
         <v>14</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="J17" s="18" t="s">
+        <v>235</v>
+      </c>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
-      <c r="M17" s="19" t="s">
-        <v>250</v>
+      <c r="M17" s="21" t="s">
+        <v>245</v>
       </c>
       <c r="N17" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D18" s="17">
         <v>1</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>238</v>
-      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
-      <c r="M18" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="N18" s="115" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="109" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="110" t="s">
+      <c r="M18" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="N18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="111" t="s">
-        <v>186</v>
-      </c>
-      <c r="D19" s="112">
-        <v>1</v>
-      </c>
-      <c r="E19" s="111" t="s">
+      <c r="C19" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="N19" s="115" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="109" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="110" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="111" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="112">
+        <v>1</v>
+      </c>
+      <c r="E20" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="113" t="s">
+      <c r="F20" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="113"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113" t="s">
-        <v>237</v>
-      </c>
-      <c r="K19" s="113" t="s">
+      <c r="G20" s="113"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113" t="s">
+        <v>235</v>
+      </c>
+      <c r="K20" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="113" t="s">
-        <v>229</v>
-      </c>
-      <c r="M19" s="114" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="D20" s="17">
-        <v>1</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="M20" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="N20" t="s">
-        <v>24</v>
+      <c r="L20" s="113" t="s">
+        <v>227</v>
+      </c>
+      <c r="M20" s="114" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3145,38 +3144,42 @@
         <v>60</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
       <c r="D21" s="17">
         <v>1</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="21" t="s">
-        <v>256</v>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>251</v>
       </c>
       <c r="N21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>235</v>
+        <v>186</v>
       </c>
       <c r="D22" s="17">
         <v>1</v>
@@ -3190,49 +3193,44 @@
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
       <c r="M22" s="21" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="N22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
       <c r="D23" s="17">
         <v>1</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18" t="s">
-        <v>237</v>
-      </c>
+      <c r="I23" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="J23" s="18"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="M23" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="N23" t="s">
-        <v>19</v>
+      <c r="L23" s="18"/>
+      <c r="M23" s="21" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3240,30 +3238,30 @@
         <v>60</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>176</v>
+        <v>233</v>
+      </c>
+      <c r="D24" s="17">
+        <v>1</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18" t="s">
-        <v>237</v>
-      </c>
+      <c r="I24" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="J24" s="18"/>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
-      <c r="M24" s="19" t="s">
-        <v>259</v>
+      <c r="M24" s="21" t="s">
+        <v>253</v>
       </c>
       <c r="N24" t="s">
-        <v>260</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3271,27 +3269,29 @@
         <v>60</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>190</v>
+        <v>242</v>
       </c>
       <c r="D25" s="17">
         <v>1</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
-      <c r="I25" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="J25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18" t="s">
+        <v>235</v>
+      </c>
       <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
+      <c r="L25" s="18" t="s">
+        <v>234</v>
+      </c>
       <c r="M25" s="19" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="N25" t="s">
         <v>19</v>
@@ -3302,28 +3302,30 @@
         <v>60</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D26" s="17">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>241</v>
+        <v>14</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
+      <c r="J26" s="18" t="s">
+        <v>235</v>
+      </c>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
       <c r="M26" s="19" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="N26" t="s">
-        <v>19</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3331,30 +3333,30 @@
         <v>60</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D27" s="17">
         <v>1</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>242</v>
+        <v>22</v>
       </c>
       <c r="F27" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G27" s="18"/>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="18"/>
+      <c r="I27" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
-      <c r="M27" s="21" t="s">
-        <v>263</v>
+      <c r="M27" s="19" t="s">
+        <v>257</v>
       </c>
       <c r="N27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3362,30 +3364,28 @@
         <v>60</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>176</v>
+        <v>190</v>
+      </c>
+      <c r="D28" s="17">
+        <v>1</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>22</v>
+        <v>239</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
-      <c r="I28" s="18" t="s">
-        <v>267</v>
-      </c>
+      <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
       <c r="M28" s="19" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="N28" t="s">
-        <v>265</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3393,185 +3393,186 @@
         <v>60</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>176</v>
+        <v>191</v>
+      </c>
+      <c r="D29" s="17">
+        <v>1</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>22</v>
+        <v>240</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18" t="s">
-        <v>226</v>
-      </c>
+      <c r="H29" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
       <c r="M29" s="21" t="s">
-        <v>333</v>
+        <v>259</v>
+      </c>
+      <c r="N29" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
       <c r="B30" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="13">
-        <v>1</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="20" t="s">
-        <v>16</v>
+        <v>60</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="N30" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
       <c r="B31" s="11" t="s">
-        <v>194</v>
+        <v>60</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="17">
-        <v>1</v>
+        <v>192</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="18" t="s">
-        <v>237</v>
-      </c>
+      <c r="I31" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="J31" s="18"/>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
-      <c r="M31" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="N31" t="s">
-        <v>19</v>
+      <c r="M31" s="21" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="22"/>
       <c r="B32" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D32" s="17">
-        <v>1</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="N32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="13">
+        <v>1</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
       <c r="B33" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>197</v>
+        <v>12</v>
       </c>
       <c r="D33" s="17">
         <v>1</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
       <c r="I33" s="23"/>
-      <c r="J33" s="18"/>
+      <c r="J33" s="18" t="s">
+        <v>235</v>
+      </c>
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
       <c r="M33" s="19" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+      <c r="N33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="22"/>
       <c r="B34" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>276</v>
+        <v>195</v>
       </c>
       <c r="D34" s="17">
         <v>1</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="G34" s="18"/>
       <c r="H34" s="18"/>
       <c r="I34" s="23"/>
       <c r="J34" s="18" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="19" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="22"/>
       <c r="B35" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>199</v>
+        <v>271</v>
       </c>
       <c r="D35" s="17">
         <v>1</v>
@@ -3583,26 +3584,26 @@
         <v>18</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>278</v>
+        <v>29</v>
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="23"/>
       <c r="J35" s="18" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="K35" s="18"/>
       <c r="L35" s="18"/>
       <c r="M35" s="19" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="22"/>
       <c r="B36" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D36" s="17">
         <v>1</v>
@@ -3614,26 +3615,26 @@
         <v>18</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
       <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
+      <c r="I36" s="23"/>
       <c r="J36" s="18" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
-      <c r="M36" s="21" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M36" s="19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="22"/>
       <c r="B37" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D37" s="17">
         <v>1</v>
@@ -3642,122 +3643,124 @@
         <v>26</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>279</v>
+        <v>328</v>
       </c>
       <c r="H37" s="18"/>
       <c r="I37" s="18"/>
       <c r="J37" s="18" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="K37" s="18"/>
       <c r="L37" s="18"/>
       <c r="M37" s="21" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="109" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="116"/>
-      <c r="B38" s="110" t="s">
-        <v>194</v>
-      </c>
-      <c r="C38" s="117" t="s">
-        <v>202</v>
-      </c>
-      <c r="D38" s="112">
-        <v>1</v>
-      </c>
-      <c r="E38" s="111" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
+      <c r="B38" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D38" s="17">
+        <v>1</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="118" t="s">
+      <c r="F38" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="H38" s="113"/>
-      <c r="I38" s="113"/>
+        <v>327</v>
+      </c>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
       <c r="J38" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K38" s="113"/>
-      <c r="L38" s="113"/>
+        <v>235</v>
+      </c>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
       <c r="M38" s="21" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="119"/>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="109" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="116"/>
       <c r="B39" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="C39" s="121" t="s">
+        <v>193</v>
+      </c>
+      <c r="C39" s="117" t="s">
+        <v>200</v>
+      </c>
+      <c r="D39" s="112">
+        <v>1</v>
+      </c>
+      <c r="E39" s="111" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="118" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="H39" s="113"/>
+      <c r="I39" s="113"/>
+      <c r="J39" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="K39" s="113"/>
+      <c r="L39" s="113"/>
+      <c r="M39" s="21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="119"/>
+      <c r="B40" s="110" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="122">
-        <v>1</v>
-      </c>
-      <c r="E39" s="121" t="s">
+      <c r="D40" s="122">
+        <v>1</v>
+      </c>
+      <c r="E40" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="123" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="123"/>
-      <c r="H39" s="123"/>
-      <c r="I39" s="123"/>
-      <c r="J39" s="123"/>
-      <c r="K39" s="123"/>
-      <c r="L39" s="123"/>
-      <c r="M39" s="20" t="s">
+      <c r="F40" s="123" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="123"/>
+      <c r="H40" s="123"/>
+      <c r="I40" s="123"/>
+      <c r="J40" s="123"/>
+      <c r="K40" s="123"/>
+      <c r="L40" s="123"/>
+      <c r="M40" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="22"/>
-      <c r="B40" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="D40" s="17">
-        <v>1</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="24" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="22"/>
       <c r="B41" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>169</v>
+        <v>265</v>
       </c>
       <c r="D41" s="17">
         <v>1</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>15</v>
@@ -3766,58 +3769,56 @@
       <c r="H41" s="18"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
-      <c r="M41" s="19" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M41" s="24" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="22"/>
       <c r="B42" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>297</v>
+        <v>169</v>
       </c>
       <c r="D42" s="17">
         <v>1</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K42" s="18"/>
-      <c r="L42" s="18" t="s">
-        <v>291</v>
-      </c>
+      <c r="L42" s="18"/>
       <c r="M42" s="19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="22"/>
       <c r="B43" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D43" s="17">
         <v>1</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>18</v>
@@ -3826,21 +3827,23 @@
       <c r="H43" s="18"/>
       <c r="I43" s="18"/>
       <c r="J43" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
+      <c r="L43" s="18" t="s">
+        <v>329</v>
+      </c>
       <c r="M43" s="19" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="22"/>
       <c r="B44" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="D44" s="17">
         <v>1</v>
@@ -3855,27 +3858,27 @@
       <c r="H44" s="18"/>
       <c r="I44" s="18"/>
       <c r="J44" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
       <c r="M44" s="19" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="22"/>
       <c r="B45" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>204</v>
+        <v>334</v>
       </c>
       <c r="D45" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>18</v>
@@ -3884,109 +3887,108 @@
       <c r="H45" s="18"/>
       <c r="I45" s="18"/>
       <c r="J45" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
-      <c r="M45" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M45" s="19" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="22"/>
       <c r="B46" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>176</v>
+        <v>202</v>
+      </c>
+      <c r="D46" s="17">
+        <v>1</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
       <c r="I46" s="18"/>
       <c r="J46" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
       <c r="M46" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="109" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="110" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="22"/>
+      <c r="B47" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="25" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="110" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="111" t="s">
         <v>203</v>
       </c>
-      <c r="C47" s="111" t="s">
-        <v>205</v>
-      </c>
-      <c r="D47" s="112">
-        <v>1</v>
-      </c>
-      <c r="E47" s="111" t="s">
+      <c r="D48" s="112">
+        <v>1</v>
+      </c>
+      <c r="E48" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="F47" s="113" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="113" t="s">
-        <v>266</v>
-      </c>
-      <c r="H47" s="113"/>
-      <c r="I47" s="113"/>
-      <c r="J47" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K47" s="113"/>
-      <c r="L47" s="113"/>
-      <c r="M47" s="125" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D48" s="17">
-        <v>1</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
+      <c r="F48" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="113" t="s">
+        <v>262</v>
+      </c>
+      <c r="H48" s="113"/>
+      <c r="I48" s="113"/>
       <c r="J48" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="26" t="s">
-        <v>281</v>
+        <v>235</v>
+      </c>
+      <c r="K48" s="113"/>
+      <c r="L48" s="113"/>
+      <c r="M48" s="125" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B49" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D49" s="17">
         <v>1</v>
@@ -3998,25 +4000,25 @@
         <v>18</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
-      <c r="M49" s="16" t="s">
-        <v>282</v>
+      <c r="M49" s="26" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B50" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D50" s="17">
         <v>1</v>
@@ -4028,53 +4030,55 @@
         <v>18</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="18"/>
       <c r="J50" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
-      <c r="M50" s="27" t="s">
-        <v>283</v>
+      <c r="M50" s="16" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B51" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D51" s="17">
         <v>1</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G51" s="18"/>
+      <c r="G51" s="18" t="s">
+        <v>279</v>
+      </c>
       <c r="H51" s="18"/>
-      <c r="I51" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="J51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18" t="s">
+        <v>235</v>
+      </c>
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
       <c r="M51" s="27" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B52" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="D52" s="17">
         <v>1</v>
@@ -4088,101 +4092,101 @@
       <c r="G52" s="18"/>
       <c r="H52" s="18"/>
       <c r="I52" s="18" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
       <c r="M52" s="27" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B53" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D53" s="17">
         <v>1</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>241</v>
+        <v>22</v>
       </c>
       <c r="F53" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G53" s="18"/>
       <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
+      <c r="I53" s="18" t="s">
+        <v>243</v>
+      </c>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
       <c r="M53" s="27" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="120" t="s">
-        <v>210</v>
-      </c>
-      <c r="C54" s="121" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B54" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="17">
+        <v>1</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="27" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B55" s="120" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="122">
-        <v>1</v>
-      </c>
-      <c r="E54" s="121" t="s">
+      <c r="D55" s="122">
+        <v>1</v>
+      </c>
+      <c r="E55" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="123" t="s">
-        <v>18</v>
-      </c>
-      <c r="G54" s="123"/>
-      <c r="H54" s="123"/>
-      <c r="I54" s="123"/>
-      <c r="J54" s="123"/>
-      <c r="K54" s="123"/>
-      <c r="L54" s="123"/>
-      <c r="M54" s="20" t="s">
+      <c r="F55" s="123" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="123"/>
+      <c r="H55" s="123"/>
+      <c r="I55" s="123"/>
+      <c r="J55" s="123"/>
+      <c r="K55" s="123"/>
+      <c r="L55" s="123"/>
+      <c r="M55" s="20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B55" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="D55" s="17">
-        <v>1</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F55" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="16" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B56" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>178</v>
+        <v>289</v>
       </c>
       <c r="D56" s="17">
         <v>1</v>
@@ -4197,26 +4201,26 @@
       <c r="H56" s="18"/>
       <c r="I56" s="18"/>
       <c r="J56" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
-      <c r="M56" s="27" t="s">
-        <v>301</v>
+      <c r="M56" s="16" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B57" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
       <c r="D57" s="17">
         <v>1</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="F57" s="18" t="s">
         <v>18</v>
@@ -4225,31 +4229,29 @@
       <c r="H57" s="18"/>
       <c r="I57" s="18"/>
       <c r="J57" s="18" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="K57" s="18"/>
-      <c r="L57" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="M57" s="16" t="s">
-        <v>302</v>
+      <c r="L57" s="18"/>
+      <c r="M57" s="27" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B58" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D58" s="17">
         <v>1</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G58" s="18"/>
       <c r="H58" s="18"/>
@@ -4258,30 +4260,30 @@
         <v>25</v>
       </c>
       <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
-      <c r="M58" s="5" t="s">
-        <v>304</v>
+      <c r="L58" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="M58" s="16" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B59" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C59" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C59" s="16" t="s">
-        <v>213</v>
-      </c>
       <c r="D59" s="17">
         <v>1</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F59" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G59" s="18" t="s">
-        <v>306</v>
-      </c>
+      <c r="G59" s="18"/>
       <c r="H59" s="18"/>
       <c r="I59" s="18"/>
       <c r="J59" s="18" t="s">
@@ -4289,28 +4291,28 @@
       </c>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
-      <c r="M59" s="16" t="s">
-        <v>305</v>
+      <c r="M59" s="5" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B60" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="D60" s="17">
         <v>1</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F60" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H60" s="18"/>
       <c r="I60" s="18"/>
@@ -4319,27 +4321,29 @@
       </c>
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
-      <c r="M60" s="27" t="s">
-        <v>307</v>
+      <c r="M60" s="16" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B61" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="D61" s="17">
         <v>1</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F61" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G61" s="18"/>
+      <c r="G61" s="18" t="s">
+        <v>296</v>
+      </c>
       <c r="H61" s="18"/>
       <c r="I61" s="18"/>
       <c r="J61" s="18" t="s">
@@ -4347,16 +4351,16 @@
       </c>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
-      <c r="M61" s="16" t="s">
-        <v>308</v>
+      <c r="M61" s="27" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B62" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D62" s="17">
         <v>1</v>
@@ -4375,16 +4379,16 @@
       </c>
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
-      <c r="M62" s="27" t="s">
-        <v>311</v>
+      <c r="M62" s="16" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B63" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D63" s="17">
         <v>1</v>
@@ -4403,29 +4407,27 @@
       </c>
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
-      <c r="M63" s="16" t="s">
-        <v>312</v>
+      <c r="M63" s="27" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B64" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D64" s="17">
         <v>1</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F64" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G64" s="18" t="s">
-        <v>306</v>
-      </c>
+      <c r="G64" s="18"/>
       <c r="H64" s="18"/>
       <c r="I64" s="18"/>
       <c r="J64" s="18" t="s">
@@ -4434,27 +4436,27 @@
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
       <c r="M64" s="16" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B65" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D65" s="17">
         <v>1</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F65" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
@@ -4464,67 +4466,71 @@
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
       <c r="M65" s="16" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B66" s="110" t="s">
-        <v>219</v>
-      </c>
-      <c r="C66" s="121" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B66" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D66" s="17">
+        <v>1</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B67" s="110" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="D66" s="122">
-        <v>1</v>
-      </c>
-      <c r="E66" s="121" t="s">
+      <c r="D67" s="122">
+        <v>1</v>
+      </c>
+      <c r="E67" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="123" t="s">
+      <c r="F67" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="123"/>
-      <c r="H66" s="123"/>
-      <c r="I66" s="123"/>
-      <c r="J66" s="123"/>
-      <c r="K66" s="123"/>
-      <c r="L66" s="123"/>
-      <c r="M66" s="20" t="s">
+      <c r="G67" s="123"/>
+      <c r="H67" s="123"/>
+      <c r="I67" s="123"/>
+      <c r="J67" s="123"/>
+      <c r="K67" s="123"/>
+      <c r="L67" s="123"/>
+      <c r="M67" s="20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B67" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="D67" s="17">
-        <v>1</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="18"/>
-      <c r="M67" s="27" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B68" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="D68" s="17">
         <v>1</v>
@@ -4541,78 +4547,76 @@
       <c r="J68" s="18"/>
       <c r="K68" s="18"/>
       <c r="L68" s="18"/>
-      <c r="M68" s="16" t="s">
-        <v>318</v>
+      <c r="M68" s="27" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B69" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>222</v>
+        <v>12</v>
       </c>
       <c r="D69" s="17">
         <v>1</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F69" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G69" s="18"/>
       <c r="H69" s="18"/>
-      <c r="I69" s="18" t="s">
-        <v>267</v>
-      </c>
+      <c r="I69" s="18"/>
       <c r="J69" s="18"/>
       <c r="K69" s="18"/>
       <c r="L69" s="18"/>
       <c r="M69" s="16" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B70" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D70" s="17">
         <v>1</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G70" s="18"/>
       <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
+      <c r="I70" s="18" t="s">
+        <v>263</v>
+      </c>
       <c r="J70" s="18"/>
       <c r="K70" s="18"/>
-      <c r="L70" s="18" t="s">
-        <v>334</v>
-      </c>
+      <c r="L70" s="18"/>
       <c r="M70" s="16" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B71" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="C71" s="16" t="s">
-        <v>223</v>
-      </c>
       <c r="D71" s="17">
         <v>1</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="F71" s="18" t="s">
         <v>15</v>
@@ -4622,77 +4626,79 @@
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
       <c r="K71" s="18"/>
-      <c r="L71" s="18"/>
-      <c r="M71" s="27" t="s">
-        <v>321</v>
+      <c r="L71" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="M71" s="16" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B72" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="D72" s="17">
         <v>1</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F72" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G72" s="18"/>
       <c r="H72" s="18"/>
-      <c r="I72" s="18" t="s">
-        <v>245</v>
-      </c>
+      <c r="I72" s="18"/>
       <c r="J72" s="18"/>
       <c r="K72" s="18"/>
       <c r="L72" s="18"/>
-      <c r="M72" s="16" t="s">
-        <v>323</v>
+      <c r="M72" s="27" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B73" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="D73" s="17">
         <v>1</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>241</v>
+        <v>22</v>
       </c>
       <c r="F73" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
+      <c r="I73" s="18" t="s">
+        <v>243</v>
+      </c>
       <c r="J73" s="18"/>
       <c r="K73" s="18"/>
       <c r="L73" s="18"/>
       <c r="M73" s="16" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B74" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D74" s="17">
         <v>1</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>15</v>
@@ -4704,69 +4710,67 @@
       <c r="K74" s="18"/>
       <c r="L74" s="18"/>
       <c r="M74" s="16" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" s="126" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="110" t="s">
-        <v>226</v>
-      </c>
-      <c r="C75" s="127" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B75" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" s="17">
+        <v>1</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F75" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="18"/>
+      <c r="M75" s="16" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" s="126" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B76" s="110" t="s">
+        <v>224</v>
+      </c>
+      <c r="C76" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D75" s="128">
-        <v>1</v>
-      </c>
-      <c r="E75" s="127" t="s">
+      <c r="D76" s="128">
+        <v>1</v>
+      </c>
+      <c r="E76" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="F75" s="129" t="s">
+      <c r="F76" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="G75" s="129"/>
-      <c r="H75" s="129"/>
-      <c r="I75" s="129"/>
-      <c r="J75" s="129"/>
-      <c r="K75" s="129"/>
-      <c r="L75" s="129"/>
-      <c r="M75" s="20" t="s">
+      <c r="G76" s="129"/>
+      <c r="H76" s="129"/>
+      <c r="I76" s="129"/>
+      <c r="J76" s="129"/>
+      <c r="K76" s="129"/>
+      <c r="L76" s="129"/>
+      <c r="M76" s="20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B76" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="D76" s="17">
-        <v>1</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F76" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-      <c r="L76" s="18"/>
-      <c r="M76" s="16" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B77" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>332</v>
+        <v>194</v>
       </c>
       <c r="D77" s="17">
         <v>1</v>
@@ -4780,53 +4784,55 @@
       <c r="G77" s="18"/>
       <c r="H77" s="18"/>
       <c r="I77" s="18" t="s">
-        <v>219</v>
+        <v>312</v>
       </c>
       <c r="J77" s="18"/>
       <c r="K77" s="18"/>
       <c r="L77" s="18"/>
       <c r="M77" s="16" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B78" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D78" s="17">
         <v>1</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G78" s="18"/>
       <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
+      <c r="I78" s="18" t="s">
+        <v>217</v>
+      </c>
       <c r="J78" s="18"/>
       <c r="K78" s="18"/>
       <c r="L78" s="18"/>
       <c r="M78" s="16" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B79" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>227</v>
+        <v>319</v>
       </c>
       <c r="D79" s="17">
         <v>1</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F79" s="18" t="s">
         <v>15</v>
@@ -4837,22 +4843,22 @@
       <c r="J79" s="18"/>
       <c r="K79" s="18"/>
       <c r="L79" s="18"/>
-      <c r="M79" s="27" t="s">
-        <v>330</v>
+      <c r="M79" s="16" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B80" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D80" s="17">
         <v>1</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>241</v>
+        <v>31</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>15</v>
@@ -4863,70 +4869,68 @@
       <c r="J80" s="18"/>
       <c r="K80" s="18"/>
       <c r="L80" s="18"/>
-      <c r="M80" s="16" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13" s="126" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="110" t="s">
-        <v>267</v>
-      </c>
-      <c r="C81" s="127" t="s">
+      <c r="M80" s="27" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B81" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D81" s="17">
+        <v>1</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F81" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13" s="126" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="C82" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D81" s="128">
-        <v>1</v>
-      </c>
-      <c r="E81" s="127" t="s">
+      <c r="D82" s="128">
+        <v>1</v>
+      </c>
+      <c r="E82" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="F81" s="129" t="s">
+      <c r="F82" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="G81" s="129"/>
-      <c r="H81" s="129"/>
-      <c r="I81" s="129"/>
-      <c r="J81" s="129"/>
-      <c r="K81" s="129"/>
-      <c r="L81" s="129"/>
-      <c r="M81" s="130" t="s">
+      <c r="G82" s="129"/>
+      <c r="H82" s="129"/>
+      <c r="I82" s="129"/>
+      <c r="J82" s="129"/>
+      <c r="K82" s="129"/>
+      <c r="L82" s="129"/>
+      <c r="M82" s="130" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B82" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="C82" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="D82" s="17">
-        <v>1</v>
-      </c>
-      <c r="E82" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
-      <c r="J82" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K82" s="18"/>
-      <c r="L82" s="18"/>
-      <c r="M82" s="16" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B83" s="11" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>268</v>
+        <v>289</v>
       </c>
       <c r="D83" s="17">
         <v>1</v>
@@ -4935,26 +4939,26 @@
         <v>14</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G83" s="18"/>
       <c r="H83" s="18"/>
       <c r="I83" s="18"/>
       <c r="J83" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K83" s="18"/>
       <c r="L83" s="18"/>
       <c r="M83" s="16" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B84" s="11" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D84" s="17">
         <v>1</v>
@@ -4969,20 +4973,20 @@
       <c r="H84" s="18"/>
       <c r="I84" s="18"/>
       <c r="J84" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K84" s="18"/>
       <c r="L84" s="18"/>
       <c r="M84" s="16" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B85" s="11" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>166</v>
+        <v>266</v>
       </c>
       <c r="D85" s="17">
         <v>1</v>
@@ -4997,12 +5001,40 @@
       <c r="H85" s="18"/>
       <c r="I85" s="18"/>
       <c r="J85" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K85" s="18"/>
       <c r="L85" s="18"/>
       <c r="M85" s="16" t="s">
-        <v>316</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B86" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D86" s="17">
+        <v>1</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="K86" s="18"/>
+      <c r="L86" s="18"/>
+      <c r="M86" s="16" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -6214,37 +6246,37 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="133" t="s">
+      <c r="B47" s="134" t="s">
         <v>126</v>
       </c>
-      <c r="C47" s="133"/>
-      <c r="D47" s="133"/>
-      <c r="E47" s="133"/>
-      <c r="F47" s="133"/>
-      <c r="H47" s="134" t="s">
+      <c r="C47" s="134"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="134"/>
+      <c r="F47" s="134"/>
+      <c r="H47" s="135" t="s">
         <v>127</v>
       </c>
-      <c r="I47" s="134"/>
+      <c r="I47" s="135"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="133"/>
-      <c r="C48" s="133"/>
-      <c r="D48" s="133"/>
-      <c r="E48" s="133"/>
-      <c r="F48" s="133"/>
-      <c r="H48" s="134"/>
-      <c r="I48" s="134"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="134"/>
+      <c r="F48" s="134"/>
+      <c r="H48" s="135"/>
+      <c r="I48" s="135"/>
     </row>
     <row r="49" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="C49" s="135" t="s">
+      <c r="C49" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="135"/>
-      <c r="E49" s="135"/>
-      <c r="F49" s="135"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="136"/>
+      <c r="F49" s="136"/>
       <c r="H49" s="80" t="s">
         <v>129</v>
       </c>
@@ -6256,12 +6288,12 @@
       <c r="B50" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="136" t="s">
+      <c r="C50" s="137" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="136"/>
-      <c r="E50" s="136"/>
-      <c r="F50" s="136"/>
+      <c r="D50" s="137"/>
+      <c r="E50" s="137"/>
+      <c r="F50" s="137"/>
       <c r="H50" s="83" t="s">
         <v>53</v>
       </c>
@@ -6273,12 +6305,12 @@
       <c r="B51" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="137" t="s">
+      <c r="C51" s="138" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="137"/>
-      <c r="E51" s="137"/>
-      <c r="F51" s="137"/>
+      <c r="D51" s="138"/>
+      <c r="E51" s="138"/>
+      <c r="F51" s="138"/>
       <c r="H51" s="86" t="s">
         <v>75</v>
       </c>
@@ -6290,12 +6322,12 @@
       <c r="B52" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="137" t="s">
+      <c r="C52" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="137"/>
-      <c r="E52" s="137"/>
-      <c r="F52" s="137"/>
+      <c r="D52" s="138"/>
+      <c r="E52" s="138"/>
+      <c r="F52" s="138"/>
       <c r="H52" s="88" t="s">
         <v>136</v>
       </c>
@@ -6307,12 +6339,12 @@
       <c r="B53" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="138" t="s">
+      <c r="C53" s="139" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="138"/>
-      <c r="E53" s="138"/>
-      <c r="F53" s="138"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="139"/>
+      <c r="F53" s="139"/>
       <c r="H53" s="88" t="s">
         <v>86</v>
       </c>
@@ -6324,12 +6356,12 @@
       <c r="B54" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="137" t="s">
+      <c r="C54" s="138" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="137"/>
-      <c r="E54" s="137"/>
-      <c r="F54" s="137"/>
+      <c r="D54" s="138"/>
+      <c r="E54" s="138"/>
+      <c r="F54" s="138"/>
       <c r="H54" s="88" t="s">
         <v>60</v>
       </c>
@@ -6341,12 +6373,12 @@
       <c r="B55" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="138" t="s">
+      <c r="C55" s="139" t="s">
         <v>142</v>
       </c>
-      <c r="D55" s="138"/>
-      <c r="E55" s="138"/>
-      <c r="F55" s="138"/>
+      <c r="D55" s="139"/>
+      <c r="E55" s="139"/>
+      <c r="F55" s="139"/>
       <c r="H55" s="90" t="s">
         <v>119</v>
       </c>
@@ -6358,67 +6390,67 @@
       <c r="B56" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="137" t="s">
+      <c r="C56" s="138" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="137"/>
-      <c r="E56" s="137"/>
-      <c r="F56" s="137"/>
+      <c r="D56" s="138"/>
+      <c r="E56" s="138"/>
+      <c r="F56" s="138"/>
     </row>
     <row r="57" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="137" t="s">
+      <c r="C57" s="138" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="137"/>
-      <c r="E57" s="137"/>
-      <c r="F57" s="137"/>
+      <c r="D57" s="138"/>
+      <c r="E57" s="138"/>
+      <c r="F57" s="138"/>
     </row>
     <row r="58" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="137" t="s">
+      <c r="C58" s="138" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="137"/>
-      <c r="E58" s="137"/>
-      <c r="F58" s="137"/>
+      <c r="D58" s="138"/>
+      <c r="E58" s="138"/>
+      <c r="F58" s="138"/>
     </row>
     <row r="59" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="137" t="s">
+      <c r="C59" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="137"/>
-      <c r="E59" s="137"/>
-      <c r="F59" s="137"/>
+      <c r="D59" s="138"/>
+      <c r="E59" s="138"/>
+      <c r="F59" s="138"/>
     </row>
     <row r="60" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="137" t="s">
+      <c r="C60" s="138" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="137"/>
-      <c r="E60" s="137"/>
-      <c r="F60" s="137"/>
+      <c r="D60" s="138"/>
+      <c r="E60" s="138"/>
+      <c r="F60" s="138"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="139" t="s">
+      <c r="C61" s="140" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="139"/>
-      <c r="E61" s="139"/>
-      <c r="F61" s="139"/>
+      <c r="D61" s="140"/>
+      <c r="E61" s="140"/>
+      <c r="F61" s="140"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="EAttMbwrYpwG6akiV7biz2nw7wlXtTooCxJogsSt7negKq0wKQ9sygPbVeHZ99cgmdNfAtLu9NnPC64y/Uaw7A==" saltValue="FJhchlgDftI44klS+XpFDg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
Added new key for userform
</commit_message>
<xml_diff>
--- a/Schema/DB_scheme.xlsx
+++ b/Schema/DB_scheme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksam432/Documents/GitHub/WP3/Schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEA8F49-4E81-8E4D-89F6-1FAC49B0CD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572041DA-4B45-C440-AE73-E968EFC1EBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="339">
   <si>
     <t>PROJET :</t>
   </si>
@@ -1049,6 +1049,12 @@
   </si>
   <si>
     <t>str/file</t>
+  </si>
+  <si>
+    <t>userForm</t>
+  </si>
+  <si>
+    <t>The filled canonical form</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2140,33 +2146,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2188,6 +2167,34 @@
     <xf numFmtId="49" fontId="1" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in 20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2619,10 +2626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:N85"/>
+  <dimension ref="A2:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2646,21 +2653,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="133" t="s">
+      <c r="C2" s="141"/>
+      <c r="D2" s="142" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -3412,34 +3419,34 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="148" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="143" t="s">
+    <row r="29" spans="1:14" s="139" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="144" t="s">
+      <c r="C29" s="135" t="s">
         <v>305</v>
       </c>
-      <c r="D29" s="145">
+      <c r="D29" s="136">
         <v>10</v>
       </c>
-      <c r="E29" s="144" t="s">
+      <c r="E29" s="135" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="146" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="146"/>
-      <c r="H29" s="146" t="s">
+      <c r="F29" s="137" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="137"/>
+      <c r="H29" s="137" t="s">
         <v>308</v>
       </c>
-      <c r="I29" s="146"/>
-      <c r="J29" s="146"/>
-      <c r="K29" s="146"/>
-      <c r="L29" s="146"/>
-      <c r="M29" s="149" t="s">
+      <c r="I29" s="137"/>
+      <c r="J29" s="137"/>
+      <c r="K29" s="137"/>
+      <c r="L29" s="137"/>
+      <c r="M29" s="140" t="s">
         <v>219</v>
       </c>
-      <c r="N29" s="148" t="s">
+      <c r="N29" s="139" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3624,7 +3631,7 @@
       <c r="B36" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="C36" s="141" t="s">
+      <c r="C36" s="132" t="s">
         <v>311</v>
       </c>
       <c r="D36" s="17">
@@ -3859,32 +3866,32 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="148" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="142"/>
-      <c r="B44" s="143" t="s">
+    <row r="44" spans="1:14" s="139" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="133"/>
+      <c r="B44" s="134" t="s">
         <v>180</v>
       </c>
-      <c r="C44" s="144" t="s">
+      <c r="C44" s="135" t="s">
         <v>315</v>
       </c>
-      <c r="D44" s="145">
-        <v>1</v>
-      </c>
-      <c r="E44" s="144" t="s">
+      <c r="D44" s="136">
+        <v>1</v>
+      </c>
+      <c r="E44" s="135" t="s">
         <v>336</v>
       </c>
-      <c r="F44" s="146" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="146"/>
-      <c r="H44" s="146"/>
-      <c r="I44" s="146"/>
-      <c r="J44" s="146" t="s">
+      <c r="F44" s="137" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="137"/>
+      <c r="H44" s="137"/>
+      <c r="I44" s="137"/>
+      <c r="J44" s="137" t="s">
         <v>198</v>
       </c>
-      <c r="K44" s="146"/>
-      <c r="L44" s="146"/>
-      <c r="M44" s="147" t="s">
+      <c r="K44" s="137"/>
+      <c r="L44" s="137"/>
+      <c r="M44" s="138" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4123,32 +4130,30 @@
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B53" s="11" t="s">
+    <row r="53" spans="2:13" s="139" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="134" t="s">
         <v>180</v>
       </c>
-      <c r="C53" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="D53" s="17">
-        <v>1</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="27" t="s">
-        <v>240</v>
+      <c r="C53" s="135" t="s">
+        <v>337</v>
+      </c>
+      <c r="D53" s="136">
+        <v>1</v>
+      </c>
+      <c r="E53" s="135" t="s">
+        <v>54</v>
+      </c>
+      <c r="F53" s="137" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="137"/>
+      <c r="H53" s="137"/>
+      <c r="I53" s="137"/>
+      <c r="J53" s="137"/>
+      <c r="K53" s="137"/>
+      <c r="L53" s="137"/>
+      <c r="M53" s="150" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.2">
@@ -4156,79 +4161,79 @@
         <v>180</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="D54" s="17">
         <v>1</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="F54" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G54" s="18"/>
       <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
+      <c r="I54" s="18" t="s">
+        <v>203</v>
+      </c>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
       <c r="M54" s="27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B55" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="D55" s="17">
+        <v>1</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="27" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="55" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="120" t="s">
+    <row r="56" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B56" s="120" t="s">
         <v>181</v>
       </c>
-      <c r="C55" s="121" t="s">
+      <c r="C56" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="D55" s="122">
-        <v>1</v>
-      </c>
-      <c r="E55" s="121" t="s">
+      <c r="D56" s="122">
+        <v>1</v>
+      </c>
+      <c r="E56" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="123" t="s">
-        <v>18</v>
-      </c>
-      <c r="G55" s="123"/>
-      <c r="H55" s="123"/>
-      <c r="I55" s="123"/>
-      <c r="J55" s="123"/>
-      <c r="K55" s="123"/>
-      <c r="L55" s="123"/>
-      <c r="M55" s="20" t="s">
+      <c r="F56" s="123" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="123"/>
+      <c r="H56" s="123"/>
+      <c r="I56" s="123"/>
+      <c r="J56" s="123"/>
+      <c r="K56" s="123"/>
+      <c r="L56" s="123"/>
+      <c r="M56" s="20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B56" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="D56" s="17">
-        <v>1</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F56" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="16" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.2">
@@ -4236,7 +4241,7 @@
         <v>181</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="D57" s="17">
         <v>1</v>
@@ -4255,8 +4260,8 @@
       </c>
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
-      <c r="M57" s="27" t="s">
-        <v>249</v>
+      <c r="M57" s="16" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.2">
@@ -4264,13 +4269,13 @@
         <v>181</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>323</v>
+        <v>224</v>
       </c>
       <c r="D58" s="17">
         <v>1</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="F58" s="18" t="s">
         <v>18</v>
@@ -4279,14 +4284,12 @@
       <c r="H58" s="18"/>
       <c r="I58" s="18"/>
       <c r="J58" s="18" t="s">
-        <v>25</v>
+        <v>198</v>
       </c>
       <c r="K58" s="18"/>
-      <c r="L58" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="M58" s="16" t="s">
-        <v>250</v>
+      <c r="L58" s="18"/>
+      <c r="M58" s="27" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.2">
@@ -4294,16 +4297,16 @@
         <v>181</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>182</v>
+        <v>323</v>
       </c>
       <c r="D59" s="17">
         <v>1</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G59" s="18"/>
       <c r="H59" s="18"/>
@@ -4312,9 +4315,11 @@
         <v>25</v>
       </c>
       <c r="K59" s="18"/>
-      <c r="L59" s="18"/>
-      <c r="M59" s="5" t="s">
-        <v>252</v>
+      <c r="L59" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="M59" s="16" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
@@ -4322,20 +4327,18 @@
         <v>181</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>324</v>
+        <v>182</v>
       </c>
       <c r="D60" s="17">
         <v>1</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F60" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G60" s="18" t="s">
-        <v>254</v>
-      </c>
+      <c r="G60" s="18"/>
       <c r="H60" s="18"/>
       <c r="I60" s="18"/>
       <c r="J60" s="18" t="s">
@@ -4343,8 +4346,8 @@
       </c>
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
-      <c r="M60" s="16" t="s">
-        <v>253</v>
+      <c r="M60" s="5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
@@ -4352,13 +4355,13 @@
         <v>181</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D61" s="17">
         <v>1</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F61" s="18" t="s">
         <v>15</v>
@@ -4373,8 +4376,8 @@
       </c>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
-      <c r="M61" s="27" t="s">
-        <v>255</v>
+      <c r="M61" s="16" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.2">
@@ -4382,18 +4385,20 @@
         <v>181</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>183</v>
+        <v>325</v>
       </c>
       <c r="D62" s="17">
         <v>1</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F62" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G62" s="18"/>
+      <c r="G62" s="18" t="s">
+        <v>254</v>
+      </c>
       <c r="H62" s="18"/>
       <c r="I62" s="18"/>
       <c r="J62" s="18" t="s">
@@ -4401,8 +4406,8 @@
       </c>
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
-      <c r="M62" s="16" t="s">
-        <v>256</v>
+      <c r="M62" s="27" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.2">
@@ -4410,7 +4415,7 @@
         <v>181</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D63" s="17">
         <v>1</v>
@@ -4429,8 +4434,8 @@
       </c>
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
-      <c r="M63" s="27" t="s">
-        <v>259</v>
+      <c r="M63" s="16" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.2">
@@ -4438,7 +4443,7 @@
         <v>181</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D64" s="17">
         <v>1</v>
@@ -4457,8 +4462,8 @@
       </c>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
-      <c r="M64" s="16" t="s">
-        <v>260</v>
+      <c r="M64" s="27" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.2">
@@ -4466,20 +4471,18 @@
         <v>181</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>326</v>
+        <v>185</v>
       </c>
       <c r="D65" s="17">
         <v>1</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F65" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G65" s="18" t="s">
-        <v>254</v>
-      </c>
+      <c r="G65" s="18"/>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
       <c r="J65" s="18" t="s">
@@ -4488,7 +4491,7 @@
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
       <c r="M65" s="16" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.2">
@@ -4496,7 +4499,7 @@
         <v>181</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D66" s="17">
         <v>1</v>
@@ -4508,7 +4511,7 @@
         <v>15</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="H66" s="18"/>
       <c r="I66" s="18"/>
@@ -4518,59 +4521,63 @@
       <c r="K66" s="18"/>
       <c r="L66" s="18"/>
       <c r="M66" s="16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="D67" s="17">
+        <v>1</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="16" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="67" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B67" s="110" t="s">
+    <row r="68" spans="2:13" s="124" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B68" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="C67" s="121" t="s">
+      <c r="C68" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="D67" s="122">
-        <v>1</v>
-      </c>
-      <c r="E67" s="121" t="s">
+      <c r="D68" s="122">
+        <v>1</v>
+      </c>
+      <c r="E68" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="123" t="s">
+      <c r="F68" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="G67" s="123"/>
-      <c r="H67" s="123"/>
-      <c r="I67" s="123"/>
-      <c r="J67" s="123"/>
-      <c r="K67" s="123"/>
-      <c r="L67" s="123"/>
-      <c r="M67" s="20" t="s">
+      <c r="G68" s="123"/>
+      <c r="H68" s="123"/>
+      <c r="I68" s="123"/>
+      <c r="J68" s="123"/>
+      <c r="K68" s="123"/>
+      <c r="L68" s="123"/>
+      <c r="M68" s="20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B68" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C68" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D68" s="17">
-        <v>1</v>
-      </c>
-      <c r="E68" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-      <c r="J68" s="18"/>
-      <c r="K68" s="18"/>
-      <c r="L68" s="18"/>
-      <c r="M68" s="27" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.2">
@@ -4578,7 +4585,7 @@
         <v>186</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>12</v>
+        <v>187</v>
       </c>
       <c r="D69" s="17">
         <v>1</v>
@@ -4595,8 +4602,8 @@
       <c r="J69" s="18"/>
       <c r="K69" s="18"/>
       <c r="L69" s="18"/>
-      <c r="M69" s="16" t="s">
-        <v>265</v>
+      <c r="M69" s="27" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.2">
@@ -4604,27 +4611,25 @@
         <v>186</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>328</v>
+        <v>12</v>
       </c>
       <c r="D70" s="17">
         <v>1</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G70" s="18"/>
       <c r="H70" s="18"/>
-      <c r="I70" s="18" t="s">
-        <v>223</v>
-      </c>
+      <c r="I70" s="18"/>
       <c r="J70" s="18"/>
       <c r="K70" s="18"/>
       <c r="L70" s="18"/>
       <c r="M70" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.2">
@@ -4632,27 +4637,27 @@
         <v>186</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D71" s="17">
         <v>1</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="F71" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
+      <c r="I71" s="18" t="s">
+        <v>223</v>
+      </c>
       <c r="J71" s="18"/>
       <c r="K71" s="18"/>
-      <c r="L71" s="18" t="s">
-        <v>279</v>
-      </c>
+      <c r="L71" s="18"/>
       <c r="M71" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.2">
@@ -4660,13 +4665,13 @@
         <v>186</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D72" s="17">
         <v>1</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="F72" s="18" t="s">
         <v>15</v>
@@ -4676,9 +4681,11 @@
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
       <c r="K72" s="18"/>
-      <c r="L72" s="18"/>
-      <c r="M72" s="27" t="s">
-        <v>268</v>
+      <c r="L72" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="M72" s="16" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.2">
@@ -4686,27 +4693,25 @@
         <v>186</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="D73" s="17">
         <v>1</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F73" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="18"/>
-      <c r="I73" s="18" t="s">
-        <v>203</v>
-      </c>
+      <c r="I73" s="18"/>
       <c r="J73" s="18"/>
       <c r="K73" s="18"/>
       <c r="L73" s="18"/>
-      <c r="M73" s="16" t="s">
-        <v>270</v>
+      <c r="M73" s="27" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.2">
@@ -4714,79 +4719,79 @@
         <v>186</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="D74" s="17">
         <v>1</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
+      <c r="I74" s="18" t="s">
+        <v>203</v>
+      </c>
       <c r="J74" s="18"/>
       <c r="K74" s="18"/>
       <c r="L74" s="18"/>
       <c r="M74" s="16" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B75" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="D75" s="17">
+        <v>1</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="F75" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="18"/>
+      <c r="M75" s="16" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="2:13" s="126" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="110" t="s">
+    <row r="76" spans="2:13" s="126" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B76" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="C75" s="127" t="s">
+      <c r="C76" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D75" s="128">
-        <v>1</v>
-      </c>
-      <c r="E75" s="127" t="s">
+      <c r="D76" s="128">
+        <v>1</v>
+      </c>
+      <c r="E76" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="F75" s="129" t="s">
+      <c r="F76" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="G75" s="129"/>
-      <c r="H75" s="129"/>
-      <c r="I75" s="129"/>
-      <c r="J75" s="129"/>
-      <c r="K75" s="129"/>
-      <c r="L75" s="129"/>
-      <c r="M75" s="20" t="s">
+      <c r="G76" s="129"/>
+      <c r="H76" s="129"/>
+      <c r="I76" s="129"/>
+      <c r="J76" s="129"/>
+      <c r="K76" s="129"/>
+      <c r="L76" s="129"/>
+      <c r="M76" s="20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B76" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="D76" s="17">
-        <v>1</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F76" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-      <c r="L76" s="18"/>
-      <c r="M76" s="16" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.2">
@@ -4794,7 +4799,7 @@
         <v>188</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D77" s="17">
         <v>1</v>
@@ -4808,13 +4813,13 @@
       <c r="G77" s="18"/>
       <c r="H77" s="18"/>
       <c r="I77" s="18" t="s">
-        <v>186</v>
+        <v>269</v>
       </c>
       <c r="J77" s="18"/>
       <c r="K77" s="18"/>
       <c r="L77" s="18"/>
       <c r="M77" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.2">
@@ -4822,25 +4827,27 @@
         <v>188</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="D78" s="17">
         <v>1</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G78" s="18"/>
       <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
+      <c r="I78" s="18" t="s">
+        <v>186</v>
+      </c>
       <c r="J78" s="18"/>
       <c r="K78" s="18"/>
       <c r="L78" s="18"/>
       <c r="M78" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.2">
@@ -4848,13 +4855,13 @@
         <v>188</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>189</v>
+        <v>275</v>
       </c>
       <c r="D79" s="17">
         <v>1</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F79" s="18" t="s">
         <v>15</v>
@@ -4865,8 +4872,8 @@
       <c r="J79" s="18"/>
       <c r="K79" s="18"/>
       <c r="L79" s="18"/>
-      <c r="M79" s="27" t="s">
-        <v>276</v>
+      <c r="M79" s="16" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.2">
@@ -4874,13 +4881,13 @@
         <v>188</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>331</v>
+        <v>189</v>
       </c>
       <c r="D80" s="17">
         <v>1</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>202</v>
+        <v>31</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>15</v>
@@ -4891,62 +4898,60 @@
       <c r="J80" s="18"/>
       <c r="K80" s="18"/>
       <c r="L80" s="18"/>
-      <c r="M80" s="16" t="s">
+      <c r="M80" s="27" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B81" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="D81" s="17">
+        <v>1</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="F81" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="16" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="81" spans="2:13" s="126" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="110" t="s">
+    <row r="82" spans="2:13" s="126" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="110" t="s">
         <v>223</v>
       </c>
-      <c r="C81" s="127" t="s">
+      <c r="C82" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D81" s="128">
-        <v>1</v>
-      </c>
-      <c r="E81" s="127" t="s">
+      <c r="D82" s="128">
+        <v>1</v>
+      </c>
+      <c r="E82" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="F81" s="129" t="s">
+      <c r="F82" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="G81" s="129"/>
-      <c r="H81" s="129"/>
-      <c r="I81" s="129"/>
-      <c r="J81" s="129"/>
-      <c r="K81" s="129"/>
-      <c r="L81" s="129"/>
-      <c r="M81" s="130" t="s">
+      <c r="G82" s="129"/>
+      <c r="H82" s="129"/>
+      <c r="I82" s="129"/>
+      <c r="J82" s="129"/>
+      <c r="K82" s="129"/>
+      <c r="L82" s="129"/>
+      <c r="M82" s="130" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B82" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C82" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="D82" s="17">
-        <v>1</v>
-      </c>
-      <c r="E82" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
-      <c r="J82" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="K82" s="18"/>
-      <c r="L82" s="18"/>
-      <c r="M82" s="16" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.2">
@@ -4954,7 +4959,7 @@
         <v>223</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="D83" s="17">
         <v>1</v>
@@ -4963,7 +4968,7 @@
         <v>14</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G83" s="18"/>
       <c r="H83" s="18"/>
@@ -4974,7 +4979,7 @@
       <c r="K83" s="18"/>
       <c r="L83" s="18"/>
       <c r="M83" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.2">
@@ -4982,7 +4987,7 @@
         <v>223</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>334</v>
+        <v>224</v>
       </c>
       <c r="D84" s="17">
         <v>1</v>
@@ -5002,7 +5007,7 @@
       <c r="K84" s="18"/>
       <c r="L84" s="18"/>
       <c r="M84" s="16" t="s">
-        <v>335</v>
+        <v>262</v>
       </c>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.2">
@@ -5010,7 +5015,7 @@
         <v>223</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>166</v>
+        <v>334</v>
       </c>
       <c r="D85" s="17">
         <v>1</v>
@@ -5030,6 +5035,34 @@
       <c r="K85" s="18"/>
       <c r="L85" s="18"/>
       <c r="M85" s="16" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B86" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D86" s="17">
+        <v>1</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="K86" s="18"/>
+      <c r="L86" s="18"/>
+      <c r="M86" s="16" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6242,37 +6275,37 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="137" t="s">
+      <c r="B47" s="143" t="s">
         <v>126</v>
       </c>
-      <c r="C47" s="137"/>
-      <c r="D47" s="137"/>
-      <c r="E47" s="137"/>
-      <c r="F47" s="137"/>
-      <c r="H47" s="138" t="s">
+      <c r="C47" s="143"/>
+      <c r="D47" s="143"/>
+      <c r="E47" s="143"/>
+      <c r="F47" s="143"/>
+      <c r="H47" s="144" t="s">
         <v>127</v>
       </c>
-      <c r="I47" s="138"/>
+      <c r="I47" s="144"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="137"/>
-      <c r="C48" s="137"/>
-      <c r="D48" s="137"/>
-      <c r="E48" s="137"/>
-      <c r="F48" s="137"/>
-      <c r="H48" s="138"/>
-      <c r="I48" s="138"/>
+      <c r="B48" s="143"/>
+      <c r="C48" s="143"/>
+      <c r="D48" s="143"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="143"/>
+      <c r="H48" s="144"/>
+      <c r="I48" s="144"/>
     </row>
     <row r="49" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="C49" s="139" t="s">
+      <c r="C49" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="139"/>
-      <c r="E49" s="139"/>
-      <c r="F49" s="139"/>
+      <c r="D49" s="145"/>
+      <c r="E49" s="145"/>
+      <c r="F49" s="145"/>
       <c r="H49" s="80" t="s">
         <v>129</v>
       </c>
@@ -6284,12 +6317,12 @@
       <c r="B50" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="140" t="s">
+      <c r="C50" s="146" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="140"/>
-      <c r="E50" s="140"/>
-      <c r="F50" s="140"/>
+      <c r="D50" s="146"/>
+      <c r="E50" s="146"/>
+      <c r="F50" s="146"/>
       <c r="H50" s="83" t="s">
         <v>53</v>
       </c>
@@ -6301,12 +6334,12 @@
       <c r="B51" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="134" t="s">
+      <c r="C51" s="147" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="134"/>
-      <c r="E51" s="134"/>
-      <c r="F51" s="134"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="147"/>
+      <c r="F51" s="147"/>
       <c r="H51" s="86" t="s">
         <v>75</v>
       </c>
@@ -6318,12 +6351,12 @@
       <c r="B52" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="134" t="s">
+      <c r="C52" s="147" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="134"/>
-      <c r="E52" s="134"/>
-      <c r="F52" s="134"/>
+      <c r="D52" s="147"/>
+      <c r="E52" s="147"/>
+      <c r="F52" s="147"/>
       <c r="H52" s="88" t="s">
         <v>136</v>
       </c>
@@ -6335,12 +6368,12 @@
       <c r="B53" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="136" t="s">
+      <c r="C53" s="148" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="136"/>
-      <c r="E53" s="136"/>
-      <c r="F53" s="136"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="148"/>
+      <c r="F53" s="148"/>
       <c r="H53" s="88" t="s">
         <v>86</v>
       </c>
@@ -6352,12 +6385,12 @@
       <c r="B54" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="134" t="s">
+      <c r="C54" s="147" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="134"/>
-      <c r="E54" s="134"/>
-      <c r="F54" s="134"/>
+      <c r="D54" s="147"/>
+      <c r="E54" s="147"/>
+      <c r="F54" s="147"/>
       <c r="H54" s="88" t="s">
         <v>60</v>
       </c>
@@ -6369,12 +6402,12 @@
       <c r="B55" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="136" t="s">
+      <c r="C55" s="148" t="s">
         <v>142</v>
       </c>
-      <c r="D55" s="136"/>
-      <c r="E55" s="136"/>
-      <c r="F55" s="136"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="148"/>
+      <c r="F55" s="148"/>
       <c r="H55" s="90" t="s">
         <v>119</v>
       </c>
@@ -6386,86 +6419,86 @@
       <c r="B56" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="134" t="s">
+      <c r="C56" s="147" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="134"/>
-      <c r="E56" s="134"/>
-      <c r="F56" s="134"/>
+      <c r="D56" s="147"/>
+      <c r="E56" s="147"/>
+      <c r="F56" s="147"/>
     </row>
     <row r="57" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="134" t="s">
+      <c r="C57" s="147" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="134"/>
-      <c r="E57" s="134"/>
-      <c r="F57" s="134"/>
+      <c r="D57" s="147"/>
+      <c r="E57" s="147"/>
+      <c r="F57" s="147"/>
     </row>
     <row r="58" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="134" t="s">
+      <c r="C58" s="147" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="134"/>
-      <c r="E58" s="134"/>
-      <c r="F58" s="134"/>
+      <c r="D58" s="147"/>
+      <c r="E58" s="147"/>
+      <c r="F58" s="147"/>
     </row>
     <row r="59" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="134" t="s">
+      <c r="C59" s="147" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="134"/>
-      <c r="E59" s="134"/>
-      <c r="F59" s="134"/>
+      <c r="D59" s="147"/>
+      <c r="E59" s="147"/>
+      <c r="F59" s="147"/>
     </row>
     <row r="60" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="134" t="s">
+      <c r="C60" s="147" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="134"/>
-      <c r="E60" s="134"/>
-      <c r="F60" s="134"/>
+      <c r="D60" s="147"/>
+      <c r="E60" s="147"/>
+      <c r="F60" s="147"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="135" t="s">
+      <c r="C61" s="149" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="135"/>
-      <c r="E61" s="135"/>
-      <c r="F61" s="135"/>
+      <c r="D61" s="149"/>
+      <c r="E61" s="149"/>
+      <c r="F61" s="149"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="EAttMbwrYpwG6akiV7biz2nw7wlXtTooCxJogsSt7negKq0wKQ9sygPbVeHZ99cgmdNfAtLu9NnPC64y/Uaw7A==" saltValue="FJhchlgDftI44klS+XpFDg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="15">
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C58:F58"/>
+    <mergeCell ref="C59:F59"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C61:F61"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="C56:F56"/>
     <mergeCell ref="B47:F48"/>
     <mergeCell ref="H47:I48"/>
     <mergeCell ref="C49:F49"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C51:F51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C58:F58"/>
-    <mergeCell ref="C59:F59"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C61:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>